<commit_message>
📊 Update SwaadSutra_Daily_2026-01-26.xlsx - 2026-01-26T12:02:19.183Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-26.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-26.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,25 +450,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-26 11:12</v>
+        <v>2026-01-26 12:02</v>
       </c>
       <c r="C2" t="str">
-        <v>Priyanka Patil</v>
+        <v>Minakshi</v>
       </c>
       <c r="D2" t="str">
-        <v>A-1605</v>
+        <v>A201</v>
       </c>
       <c r="E2" t="str">
-        <v>9867003224</v>
+        <v>7387851735</v>
       </c>
       <c r="F2" t="str">
-        <v>Jawar Bhakari x2</v>
+        <v>Wheat Chapati x5</v>
       </c>
       <c r="G2">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -477,10 +477,10 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-27</v>
+        <v>2026-01-26</v>
       </c>
       <c r="K2" t="str">
-        <v>09:00</v>
+        <v>19:30</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -492,9 +492,53 @@
         <v/>
       </c>
     </row>
+    <row r="3">
+      <c r="A3">
+        <v>29</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2026-01-26 11:12</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Priyanka Patil</v>
+      </c>
+      <c r="D3" t="str">
+        <v>A-1605</v>
+      </c>
+      <c r="E3" t="str">
+        <v>9867003224</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Jawar Bhakari x2</v>
+      </c>
+      <c r="G3">
+        <v>40</v>
+      </c>
+      <c r="H3" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I3" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J3" t="str">
+        <v>2026-01-27</v>
+      </c>
+      <c r="K3" t="str">
+        <v>09:00</v>
+      </c>
+      <c r="L3" t="str">
+        <v/>
+      </c>
+      <c r="M3" t="str">
+        <v/>
+      </c>
+      <c r="N3" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N3"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -534,10 +578,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -552,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -567,7 +611,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -585,18 +629,29 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>Wheat Chapati</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
         <v>Jawar Bhakari</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-26.xlsx - 2026-01-26T15:00:31.114Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-26.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-26.xlsx
@@ -471,7 +471,7 @@
         <v>75</v>
       </c>
       <c r="H2" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -581,7 +581,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>0</v>

</xml_diff>